<commit_message>
Fix a tabla Resultados promedio
</commit_message>
<xml_diff>
--- a/Pruebas/Resumen de resultados Entrevista.xlsx
+++ b/Pruebas/Resumen de resultados Entrevista.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcand\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Godot\Godot Normal\Juego Base - ROLLBACK NETCODE\Juego Base\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E76DA3-1F90-41AB-A068-8764AC58A36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101C5687-3402-4B12-BFB2-148615BC9930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,9 +227,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -240,7 +239,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -4031,7 +4029,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CL"/>
-                  <a:t>Calificación</a:t>
+                  <a:t>Latencia (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4152,13 +4150,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CL"/>
-                  <a:t>Cantidad</a:t>
+                  <a:t>Calificación Promedio</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="es-CL" baseline="0"/>
-                  <a:t> de Personas</a:t>
-                </a:r>
-                <a:endParaRPr lang="es-CL"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4547,7 +4540,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CL"/>
-                  <a:t>Calificación</a:t>
+                  <a:t>Latencia (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4668,7 +4661,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CL"/>
-                  <a:t>Cantidad de Personas</a:t>
+                  <a:t>Calificación Promedio</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5063,7 +5056,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CL"/>
-                  <a:t>Calificación</a:t>
+                  <a:t>Latencia (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5184,7 +5177,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CL"/>
-                  <a:t>Cantidad de Personas</a:t>
+                  <a:t>Calificación Promedio</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -10819,8 +10812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y36" sqref="Y36"/>
+    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10838,82 +10831,82 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>2</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>3</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>4</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>5</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>6</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>7</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>8</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <v>9</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="9">
         <v>10</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-      <c r="G3" s="12">
-        <v>0</v>
-      </c>
-      <c r="H3" s="12">
-        <v>0</v>
-      </c>
-      <c r="I3" s="12">
-        <v>0</v>
-      </c>
-      <c r="J3" s="12">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
         <v>10</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="13">
+      <c r="M3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="11">
         <f>((1*B3)+(2*C3)+(3*D3)+(4*E3)+(5*F3)+(6*G3)+(7*H3)+(8*I3)+(9*J3)+(10*K3))/10</f>
         <v>10</v>
       </c>
@@ -10922,43 +10915,43 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="11">
         <f>((1*B4)+(2*C4)+(3*D4)+(4*E4)+(5*F4)+(6*G4)+(7*H4)+(8*I4)+(9*J4)+(10*K4))/10</f>
         <v>3.8</v>
       </c>
@@ -10967,43 +10960,43 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7" t="s">
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="13">
         <f>((1*B5)+(2*C5)+(3*D5)+(4*E5)+(5*F5)+(6*G5)+(7*H5)+(8*I5)+(9*J5)+(10*K5))/10</f>
         <v>1.9</v>
       </c>
@@ -11012,82 +11005,82 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>2</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>3</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>4</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>5</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>6</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>7</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <v>8</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>9</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <v>10</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="10"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="12">
-        <v>0</v>
-      </c>
-      <c r="C8" s="12">
-        <v>0</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0</v>
-      </c>
-      <c r="H8" s="12">
-        <v>0</v>
-      </c>
-      <c r="I8" s="12">
-        <v>0</v>
-      </c>
-      <c r="J8" s="12">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
         <v>10</v>
       </c>
-      <c r="M8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N8" s="14">
+      <c r="M8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12">
         <f>((1*B8)+(2*C8)+(3*D8)+(4*E8)+(5*F8)+(6*G8)+(7*H8)+(8*I8)+(9*J8)+(10*K8))/10</f>
         <v>10</v>
       </c>
@@ -11096,43 +11089,43 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="12">
-        <v>0</v>
-      </c>
-      <c r="C9" s="12">
-        <v>0</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12">
-        <v>0</v>
-      </c>
-      <c r="H9" s="12">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12">
-        <v>0</v>
-      </c>
-      <c r="J9" s="12">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
         <v>10</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="11">
         <f>((1*B9)+(2*C9)+(3*D9)+(4*E9)+(5*F9)+(6*G9)+(7*H9)+(8*I9)+(9*J9)+(10*K9))/10</f>
         <v>10</v>
       </c>
@@ -11141,43 +11134,43 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3">
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
         <v>2</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>8</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="13">
         <f>((1*B10)+(2*C10)+(3*D10)+(4*E10)+(5*F10)+(6*G10)+(7*H10)+(8*I10)+(9*J10)+(10*K10))/10</f>
         <v>9.8000000000000007</v>
       </c>
@@ -11194,82 +11187,82 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>1</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>2</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>3</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>4</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>5</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>6</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>7</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <v>8</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <v>9</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>10</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N13" s="10"/>
+      <c r="N13" s="9"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0</v>
-      </c>
-      <c r="G14" s="12">
-        <v>0</v>
-      </c>
-      <c r="H14" s="12">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
+      <c r="A14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <v>2</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14">
         <v>5</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>3</v>
       </c>
-      <c r="M14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N14" s="13">
+      <c r="M14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="11">
         <f>((1*B14)+(2*C14)+(3*D14)+(4*E14)+(5*F14)+(6*G14)+(7*H14)+(8*I14)+(9*J14)+(10*K14))/10</f>
         <v>9.1</v>
       </c>
@@ -11278,43 +11271,43 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>4</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>2</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>3</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6" t="s">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="11">
         <f>((1*B15)+(2*C15)+(3*D15)+(4*E15)+(5*F15)+(6*G15)+(7*H15)+(8*I15)+(9*J15)+(10*K15))/10</f>
         <v>4.0999999999999996</v>
       </c>
@@ -11323,43 +11316,43 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>4</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>2</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>1</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>1</v>
       </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="M16" s="7" t="s">
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="13">
         <f>((1*B16)+(2*C16)+(3*D16)+(4*E16)+(5*F16)+(6*G16)+(7*H16)+(8*I16)+(9*J16)+(10*K16))/10</f>
         <v>1.5</v>
       </c>
@@ -11368,82 +11361,82 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>1</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>2</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>3</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>4</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>5</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>6</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>7</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="8">
         <v>8</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <v>9</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <v>10</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N18" s="10"/>
+      <c r="N18" s="9"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="12">
-        <v>0</v>
-      </c>
-      <c r="C19" s="12">
-        <v>0</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0</v>
-      </c>
-      <c r="G19" s="12">
-        <v>0</v>
-      </c>
-      <c r="H19" s="12">
-        <v>0</v>
-      </c>
-      <c r="I19" s="12">
+      <c r="A19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>1</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19">
         <v>3</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <v>6</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N19" s="14">
+      <c r="M19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="12">
         <f>((1*B19)+(2*C19)+(3*D19)+(4*E19)+(5*F19)+(6*G19)+(7*H19)+(8*I19)+(9*J19)+(10*K19))/10</f>
         <v>9.5</v>
       </c>
@@ -11452,43 +11445,43 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="12">
-        <v>0</v>
-      </c>
-      <c r="C20" s="12">
-        <v>0</v>
-      </c>
-      <c r="D20" s="12">
-        <v>0</v>
-      </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0</v>
-      </c>
-      <c r="G20" s="12">
-        <v>0</v>
-      </c>
-      <c r="H20" s="12">
-        <v>0</v>
-      </c>
-      <c r="I20" s="12">
-        <v>0</v>
-      </c>
-      <c r="J20" s="12">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
         <v>4</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>6</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="M20" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="11">
         <f>((1*B20)+(2*C20)+(3*D20)+(4*E20)+(5*F20)+(6*G20)+(7*H20)+(8*I20)+(9*J20)+(10*K20))/10</f>
         <v>9.6</v>
       </c>
@@ -11497,43 +11490,43 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="3">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
         <v>1</v>
       </c>
-      <c r="I21" s="3">
-        <v>0</v>
-      </c>
-      <c r="J21" s="3">
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
         <v>4</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="3">
         <v>5</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="M21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N21" s="15">
+      <c r="N21" s="13">
         <f>((1*B21)+(2*C21)+(3*D21)+(4*E21)+(5*F21)+(6*G21)+(7*H21)+(8*I21)+(9*J21)+(10*K21))/10</f>
         <v>9.3000000000000007</v>
       </c>
@@ -11550,82 +11543,82 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="8">
         <v>1</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>2</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <v>3</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>4</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <v>5</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <v>6</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <v>7</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="8">
         <v>8</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <v>9</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="9">
         <v>10</v>
       </c>
-      <c r="M24" s="11" t="s">
+      <c r="M24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N24" s="10"/>
+      <c r="N24" s="9"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="12">
-        <v>0</v>
-      </c>
-      <c r="F25" s="12">
-        <v>0</v>
-      </c>
-      <c r="G25" s="12">
-        <v>0</v>
-      </c>
-      <c r="H25" s="12">
-        <v>0</v>
-      </c>
-      <c r="I25" s="12">
-        <v>0</v>
-      </c>
-      <c r="J25" s="12">
-        <v>0</v>
-      </c>
-      <c r="K25" s="2">
+      <c r="A25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
         <v>10</v>
       </c>
-      <c r="M25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N25" s="13">
+      <c r="M25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="11">
         <f>((1*B25)+(2*C25)+(3*D25)+(4*E25)+(5*F25)+(6*G25)+(7*H25)+(8*I25)+(9*J25)+(10*K25))/10</f>
         <v>10</v>
       </c>
@@ -11634,43 +11627,43 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
         <v>3</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26">
         <v>6</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26">
         <v>1</v>
       </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0</v>
-      </c>
-      <c r="M26" s="6" t="s">
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N26" s="13">
+      <c r="N26" s="11">
         <f>((1*B26)+(2*C26)+(3*D26)+(4*E26)+(5*F26)+(6*G26)+(7*H26)+(8*I26)+(9*J26)+(10*K26))/10</f>
         <v>4.8</v>
       </c>
@@ -11679,43 +11672,43 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>5</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>2</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>3</v>
       </c>
-      <c r="E27" s="3">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
-        <v>0</v>
-      </c>
-      <c r="J27" s="3">
-        <v>0</v>
-      </c>
-      <c r="K27" s="4">
-        <v>0</v>
-      </c>
-      <c r="M27" s="7" t="s">
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="M27" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N27" s="15">
+      <c r="N27" s="13">
         <f>((1*B27)+(2*C27)+(3*D27)+(4*E27)+(5*F27)+(6*G27)+(7*H27)+(8*I27)+(9*J27)+(10*K27))/10</f>
         <v>1.8</v>
       </c>
@@ -11724,82 +11717,82 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="7">
         <v>1</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>2</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="8">
         <v>3</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="8">
         <v>4</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="8">
         <v>5</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="8">
         <v>6</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="8">
         <v>7</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="8">
         <v>8</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="8">
         <v>9</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="9">
         <v>10</v>
       </c>
-      <c r="M29" s="11" t="s">
+      <c r="M29" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="N29" s="10"/>
+      <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="12">
-        <v>0</v>
-      </c>
-      <c r="C30" s="12">
-        <v>0</v>
-      </c>
-      <c r="D30" s="12">
-        <v>0</v>
-      </c>
-      <c r="E30" s="12">
-        <v>0</v>
-      </c>
-      <c r="F30" s="12">
-        <v>0</v>
-      </c>
-      <c r="G30" s="12">
-        <v>0</v>
-      </c>
-      <c r="H30" s="12">
-        <v>0</v>
-      </c>
-      <c r="I30" s="12">
-        <v>0</v>
-      </c>
-      <c r="J30" s="12">
+      <c r="A30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
         <v>1</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="1">
         <v>9</v>
       </c>
-      <c r="M30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N30" s="14">
+      <c r="M30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" s="12">
         <f>((1*B30)+(2*C30)+(3*D30)+(4*E30)+(5*F30)+(6*G30)+(7*H30)+(8*I30)+(9*J30)+(10*K30))/10</f>
         <v>9.9</v>
       </c>
@@ -11808,43 +11801,43 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="12">
-        <v>0</v>
-      </c>
-      <c r="C31" s="12">
-        <v>0</v>
-      </c>
-      <c r="D31" s="12">
-        <v>0</v>
-      </c>
-      <c r="E31" s="12">
-        <v>0</v>
-      </c>
-      <c r="F31" s="12">
-        <v>0</v>
-      </c>
-      <c r="G31" s="12">
-        <v>0</v>
-      </c>
-      <c r="H31" s="12">
-        <v>0</v>
-      </c>
-      <c r="I31" s="12">
-        <v>0</v>
-      </c>
-      <c r="J31" s="12">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
         <v>1</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="1">
         <v>9</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="M31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N31" s="13">
+      <c r="N31" s="11">
         <f>((1*B31)+(2*C31)+(3*D31)+(4*E31)+(5*F31)+(6*G31)+(7*H31)+(8*I31)+(9*J31)+(10*K31))/10</f>
         <v>9.9</v>
       </c>
@@ -11853,43 +11846,43 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="3">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
         <v>1</v>
       </c>
-      <c r="H32" s="3">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3">
-        <v>0</v>
-      </c>
-      <c r="J32" s="3">
-        <v>0</v>
-      </c>
-      <c r="K32" s="4">
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
         <v>9</v>
       </c>
-      <c r="M32" s="7" t="s">
+      <c r="M32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N32" s="15">
+      <c r="N32" s="13">
         <f>((1*B32)+(2*C32)+(3*D32)+(4*E32)+(5*F32)+(6*G32)+(7*H32)+(8*I32)+(9*J32)+(10*K32))/10</f>
         <v>9.6</v>
       </c>

</xml_diff>